<commit_message>
made figure of otocatch vs CPUE , but 2021 looks wonky
</commit_message>
<xml_diff>
--- a/Data/CPUE/2019_Yukon_expanded_CPUE.xlsx
+++ b/Data/CPUE/2019_Yukon_expanded_CPUE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmakhlouf/Research_repos/Shifting-Habitat-Mosaics-II/Data/CPUE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F62EFB2B-9E0C-6D44-A02E-A433A0D26D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{682DAB9D-E9AD-D045-B0DE-5FF9DE44D7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1740" windowWidth="24960" windowHeight="16260" xr2:uid="{9212F4B1-7736-E241-931B-987827C3DB4D}"/>
+    <workbookView xWindow="4440" yWindow="1240" windowWidth="24960" windowHeight="16260" xr2:uid="{9212F4B1-7736-E241-931B-987827C3DB4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -112,7 +115,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,13 +433,16 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">

</xml_diff>